<commit_message>
My work at 5 pm on Oct 3
</commit_message>
<xml_diff>
--- a/1 Shiny App/MyShinyObjects.xlsx
+++ b/1 Shiny App/MyShinyObjects.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
   <si>
     <t>global.R</t>
   </si>
@@ -72,12 +72,6 @@
     <t>trends</t>
   </si>
   <si>
-    <t>trend_countries</t>
-  </si>
-  <si>
-    <t>trend_indicators</t>
-  </si>
-  <si>
     <t>Vector of indicator names - for user to select indicator for trends</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t xml:space="preserve">      selectizeInput: map_indicator</t>
   </si>
   <si>
-    <t>User selects the indicator for trends</t>
-  </si>
-  <si>
     <t xml:space="preserve">      selectizeInput: trends_country</t>
   </si>
   <si>
@@ -250,6 +241,21 @@
   </si>
   <si>
     <t xml:space="preserve">      selectizeInput: trends_indicator1</t>
+  </si>
+  <si>
+    <t>trends_countries</t>
+  </si>
+  <si>
+    <t>trends_indicators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      selectizeInput: trends_indicator2</t>
+  </si>
+  <si>
+    <t>User selects indicator 1 for trends</t>
+  </si>
+  <si>
+    <t>User selects indicator 2 for trends</t>
   </si>
 </sst>
 </file>
@@ -1417,10 +1423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1428,6 +1434,7 @@
     <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="3.140625" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="54.28515625" customWidth="1"/>
   </cols>
@@ -1437,10 +1444,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1459,7 +1466,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -1478,7 +1485,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1522,10 +1529,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
@@ -1533,10 +1540,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
@@ -1544,35 +1551,35 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1580,56 +1587,56 @@
         <v>4</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
         <v>16</v>
@@ -1637,10 +1644,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
@@ -1648,31 +1655,31 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
         <v>16</v>
@@ -1680,159 +1687,173 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
         <v>16</v>
       </c>
-      <c r="E27" t="s">
-        <v>65</v>
-      </c>
-      <c r="F27" t="s">
-        <v>66</v>
-      </c>
       <c r="G27" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
         <v>16</v>
       </c>
-      <c r="E28" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28" t="s">
-        <v>67</v>
-      </c>
       <c r="G28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
         <v>16</v>
       </c>
-      <c r="E29" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" t="s">
-        <v>70</v>
-      </c>
       <c r="G29" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>47</v>
+      <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" t="s">
-        <v>7</v>
+        <v>16</v>
+      </c>
+      <c r="G30" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" t="s">
-        <v>55</v>
+      <c r="A32" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
       </c>
+      <c r="E32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>51</v>
-      </c>
-      <c r="B33" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
       </c>
+      <c r="E33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="6" t="s">
+      <c r="A34" t="s">
         <v>48</v>
       </c>
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>59</v>
+      </c>
+      <c r="F34" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>49</v>
       </c>
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
       <c r="C35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>57</v>
-      </c>
-      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" t="s">
+        <v>68</v>
+      </c>
+      <c r="F39" t="s">
+        <v>70</v>
+      </c>
+      <c r="G39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>58</v>
       </c>
-      <c r="C36" t="s">
-        <v>23</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="B40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" t="s">
+        <v>69</v>
+      </c>
+      <c r="F40" t="s">
         <v>71</v>
       </c>
-      <c r="F36" t="s">
-        <v>73</v>
-      </c>
-      <c r="G36" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="G40" t="s">
         <v>72</v>
-      </c>
-      <c r="F37" t="s">
-        <v>74</v>
-      </c>
-      <c r="G37" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1842,68 +1863,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f2684793-112f-4fec-9fa7-c952a73f86d3">
-      <Value>64</Value>
-      <Value>69</Value>
-      <Value>57</Value>
-      <Value>97</Value>
-      <Value>68</Value>
-      <Value>73</Value>
-    </TaxCatchAll>
-    <ProductsTaxHTField0 xmlns="72acfbc7-13d6-4e32-8fe0-794e2d8bf5d1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Not applicable</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">15480a47-f0f1-4795-a643-bf3b2e95805c</TermId>
-        </TermInfo>
-      </Terms>
-    </ProductsTaxHTField0>
-    <gNetLanguagesTaxHTField0 xmlns="92833d98-8015-4e73-bff4-7fc7bdc77146">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">English</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">914398da-6a81-430b-8d1c-6a7bd1227f71</TermId>
-        </TermInfo>
-      </Terms>
-    </gNetLanguagesTaxHTField0>
-    <IndustriesTaxHTField0 xmlns="92833d98-8015-4e73-bff4-7fc7bdc77146">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Not applicable</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">1b0d69d1-6137-41de-9ae5-e5925610d8cb</TermId>
-        </TermInfo>
-      </Terms>
-    </IndustriesTaxHTField0>
-    <ExpertContentTaxHTField0 xmlns="92833d98-8015-4e73-bff4-7fc7bdc77146">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ExpertContentTaxHTField0>
-    <FunctionalAreaTaxHTField0 xmlns="92833d98-8015-4e73-bff4-7fc7bdc77146">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </FunctionalAreaTaxHTField0>
-    <CountriesTaxHTField0 xmlns="92833d98-8015-4e73-bff4-7fc7bdc77146">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Global</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">3eaca359-c4b3-4b51-a927-e9852da92384</TermId>
-        </TermInfo>
-      </Terms>
-    </CountriesTaxHTField0>
-    <ClientsTaxHTField0 xmlns="92833d98-8015-4e73-bff4-7fc7bdc77146">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Not applicable</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">457da623-78f9-49de-8564-b1618c49ba59</TermId>
-        </TermInfo>
-      </Terms>
-    </ClientsTaxHTField0>
-    <gNetNextKeyDocument xmlns="92833d98-8015-4e73-bff4-7fc7bdc77146">No</gNetNextKeyDocument>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ExpertContentDocumentLibrary" ma:contentTypeID="0x010100D0AFC36ACFD74F7BA0C77049996D405C00FF49417D29D72E4D9B5054C9AC26121A" ma:contentTypeVersion="0" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="6360a5f94c527d9e7ec2ba7d0336b460">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="92833d98-8015-4e73-bff4-7fc7bdc77146" xmlns:ns3="72acfbc7-13d6-4e32-8fe0-794e2d8bf5d1" xmlns:ns4="f2684793-112f-4fec-9fa7-c952a73f86d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4dd616222a85d58f18a73fd7fa601ae7" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="92833d98-8015-4e73-bff4-7fc7bdc77146"/>
@@ -2122,12 +2081,69 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="8fb135ec-df78-4771-b246-ee3879de3bc6" ContentTypeId="0x010100D0AFC36ACFD74F7BA0C77049996D405C" PreviousValue="false"/>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f2684793-112f-4fec-9fa7-c952a73f86d3">
+      <Value>64</Value>
+      <Value>69</Value>
+      <Value>57</Value>
+      <Value>97</Value>
+      <Value>68</Value>
+      <Value>73</Value>
+    </TaxCatchAll>
+    <ProductsTaxHTField0 xmlns="72acfbc7-13d6-4e32-8fe0-794e2d8bf5d1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Not applicable</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">15480a47-f0f1-4795-a643-bf3b2e95805c</TermId>
+        </TermInfo>
+      </Terms>
+    </ProductsTaxHTField0>
+    <gNetLanguagesTaxHTField0 xmlns="92833d98-8015-4e73-bff4-7fc7bdc77146">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">English</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">914398da-6a81-430b-8d1c-6a7bd1227f71</TermId>
+        </TermInfo>
+      </Terms>
+    </gNetLanguagesTaxHTField0>
+    <IndustriesTaxHTField0 xmlns="92833d98-8015-4e73-bff4-7fc7bdc77146">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Not applicable</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">1b0d69d1-6137-41de-9ae5-e5925610d8cb</TermId>
+        </TermInfo>
+      </Terms>
+    </IndustriesTaxHTField0>
+    <ExpertContentTaxHTField0 xmlns="92833d98-8015-4e73-bff4-7fc7bdc77146">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ExpertContentTaxHTField0>
+    <FunctionalAreaTaxHTField0 xmlns="92833d98-8015-4e73-bff4-7fc7bdc77146">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </FunctionalAreaTaxHTField0>
+    <CountriesTaxHTField0 xmlns="92833d98-8015-4e73-bff4-7fc7bdc77146">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Global</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">3eaca359-c4b3-4b51-a927-e9852da92384</TermId>
+        </TermInfo>
+      </Terms>
+    </CountriesTaxHTField0>
+    <ClientsTaxHTField0 xmlns="92833d98-8015-4e73-bff4-7fc7bdc77146">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Not applicable</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">457da623-78f9-49de-8564-b1618c49ba59</TermId>
+        </TermInfo>
+      </Terms>
+    </ClientsTaxHTField0>
+    <gNetNextKeyDocument xmlns="92833d98-8015-4e73-bff4-7fc7bdc77146">No</gNetNextKeyDocument>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2136,25 +2152,12 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F480E75-6D1D-44D0-B504-9E00170BB20C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="92833d98-8015-4e73-bff4-7fc7bdc77146"/>
-    <ds:schemaRef ds:uri="72acfbc7-13d6-4e32-8fe0-794e2d8bf5d1"/>
-    <ds:schemaRef ds:uri="f2684793-112f-4fec-9fa7-c952a73f86d3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="8fb135ec-df78-4771-b246-ee3879de3bc6" ContentTypeId="0x010100D0AFC36ACFD74F7BA0C77049996D405C" PreviousValue="false"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{362E6889-D0FC-42B3-ADE6-8BEB21269DB6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2174,18 +2177,36 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F480E75-6D1D-44D0-B504-9E00170BB20C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="92833d98-8015-4e73-bff4-7fc7bdc77146"/>
+    <ds:schemaRef ds:uri="72acfbc7-13d6-4e32-8fe0-794e2d8bf5d1"/>
+    <ds:schemaRef ds:uri="f2684793-112f-4fec-9fa7-c952a73f86d3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDF09A26-9023-4798-A4A9-90737409C1AB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EABE0621-2CCE-4417-AFBF-BE5B8A71D39B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDF09A26-9023-4798-A4A9-90737409C1AB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>